<commit_message>
refactored + config values can now be read from excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/foo.xlsx
+++ b/src/test/resources/testdata/foo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>data.Foo</t>
   </si>
@@ -70,6 +70,9 @@
     <t>intArray</t>
   </si>
   <si>
+    <t>veryLongPropertyName</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
     <t>3,4,5</t>
   </si>
   <si>
+    <t>abc</t>
+  </si>
+  <si>
     <t>test2</t>
   </si>
   <si>
@@ -106,6 +112,9 @@
     <t>FOO_2</t>
   </si>
   <si>
+    <t>xyz</t>
+  </si>
+  <si>
     <t>data.Bar</t>
   </si>
   <si>
@@ -131,6 +140,12 @@
   </si>
   <si>
     <t>bas3</t>
+  </si>
+  <si>
+    <t>vlpn</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -147,6 +162,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,6 +184,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -233,6 +250,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -250,18 +271,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.70408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2755102040816"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.8418367346939"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +307,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -333,13 +356,16 @@
       <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>123</v>
@@ -354,42 +380,45 @@
         <v>901</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>222</v>
@@ -404,18 +433,18 @@
         <v>888</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -423,6 +452,9 @@
         <v>2</v>
       </c>
       <c r="P4" s="2"/>
+      <c r="Q4" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
@@ -462,7 +494,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -488,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -509,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>123</v>
@@ -566,7 +598,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -589,13 +621,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -618,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>1</v>
@@ -644,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>2</v>
@@ -670,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>3</v>
@@ -688,6 +720,28 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -711,6 +765,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -734,6 +791,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>